<commit_message>
Update model tuning parameters and improve rolling feature calculation
- Adjusted XGBoost parameters: increased max_depth from 4 to 5, resulting in a new best score of 50.75%.
- Updated Random Forest parameters: changed max_depth from 12 to 10 and max_features from 'sqrt' to 0.5, achieving a best score of 50.19%.
- Modified Logistic Regression best score from 49.81% to 49.43%.
- Revised calibrated accuracy from 63.14% to 61.57%.
- Enhanced rolling feature calculation by increasing the EWM span from 5 to 10.
- Updated sample probabilities and accuracy metrics for various thresholds.
- Added a new temporary Excel file for the betting slip.
</commit_message>
<xml_diff>
--- a/quant_betting_slip.xlsx
+++ b/quant_betting_slip.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Pot_Profit</t>
+          <t>Profit</t>
         </is>
       </c>
     </row>
@@ -495,10 +495,10 @@
         <v>2.53</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5604392610134347</v>
+        <v>0.537014889210818</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4179113303639896</v>
+        <v>0.3586476697033694</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -506,48 +506,48 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.06828616509215518</v>
+        <v>0.04688204832723783</v>
       </c>
       <c r="H2" t="n">
-        <v>2.048584952764656</v>
+        <v>1.406461449817135</v>
       </c>
       <c r="I2" t="n">
-        <v>5.182919930494578</v>
+        <v>2.151886018220216</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HOME</t>
+          <t>AWAY</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Burnley</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.01</v>
+        <v>4.03</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4419418967918877</v>
+        <v>0.3927878780681108</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7721870061354696</v>
+        <v>0.5829351486144867</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Burnley vs Everton</t>
+          <t>Chelsea vs Aston Villa</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.06413513339995595</v>
+        <v>0.03078205405225012</v>
       </c>
       <c r="H3" t="n">
-        <v>1.924054001998679</v>
+        <v>0.9234616215675037</v>
       </c>
       <c r="I3" t="n">
-        <v>7.715456548014701</v>
+        <v>2.798088713349536</v>
       </c>
     </row>
     <row r="4">
@@ -558,66 +558,66 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nottingham Forest</t>
+          <t>Burnley</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.29</v>
+        <v>4.01</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2783478641200504</v>
+        <v>0.3896918319201798</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4724602011950667</v>
+        <v>0.5626642459999209</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Nottingham Forest vs Manchester City</t>
+          <t>Burnley vs Everton</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.02753264575728826</v>
+        <v>0.0299090629102948</v>
       </c>
       <c r="H4" t="n">
-        <v>0.825979372718648</v>
+        <v>0.8972718873088441</v>
       </c>
       <c r="I4" t="n">
-        <v>4.369430881681648</v>
+        <v>2.70078838079962</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AWAY</t>
+          <t>HOME</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>West Ham United</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4.03</v>
+        <v>2.68</v>
       </c>
       <c r="D5" t="n">
-        <v>0.316691605089426</v>
+        <v>0.4438756880932579</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2762671685103868</v>
+        <v>0.1895868440899313</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Chelsea vs Aston Villa</t>
+          <t>West Ham United vs Fulham</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.02279432083419033</v>
+        <v>0.02256986239165849</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6838296250257099</v>
+        <v>0.6770958717497547</v>
       </c>
       <c r="I5" t="n">
-        <v>2.755833388853611</v>
+        <v>1.137521064539588</v>
       </c>
     </row>
     <row r="6">
@@ -628,66 +628,66 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>West Ham United</t>
+          <t>Nottingham Forest</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.68</v>
+        <v>5.29</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4175294587549044</v>
+        <v>0.2345800676157228</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1189789494631439</v>
+        <v>0.2409285576871736</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>West Ham United vs Fulham</t>
+          <t>Nottingham Forest vs Manchester City</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.01770520081296783</v>
+        <v>0.006739260354885974</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5311560243890348</v>
+        <v>0.2021778106465792</v>
       </c>
       <c r="I6" t="n">
-        <v>1.423498145362613</v>
+        <v>0.8673428076738249</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HOME</t>
+          <t>DRAW</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Brentford</t>
+          <t>Draw</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.29</v>
+        <v>4.92</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4687251115787607</v>
+        <v>0.2189947313686686</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07338050551536202</v>
+        <v>0.07745407833384976</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Brentford vs Bournemouth</t>
+          <t>Arsenal vs Brighton &amp; Hove Albion</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.01422102820065158</v>
+        <v>0.002371043214301524</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4266308460195473</v>
+        <v>0.07113129642904571</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9769846373847633</v>
+        <v>0.2788346820018592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>